<commit_message>
Updated MAIN excel data sheet for IC update scenario; Updated ic_ClickAndCollect to accept alert popup.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN_Backup.xlsx
+++ b/src/test/resources/data/jdgroupMAIN_Backup.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BE3CE9-EA89-4BAD-9378-109EF82E6BAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16982545-759F-47E1-9778-3613608457CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="61" activeTab="63" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
@@ -5030,17 +5030,7 @@
     <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
-  <dxfs count="530">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="529">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -10988,19 +10978,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="372" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="371" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="371" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="370" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A4">
-    <cfRule type="duplicateValues" dxfId="370" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="369" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="369" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="368" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="368" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="367" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{00000000-0002-0000-0800-000000000000}">
@@ -11466,22 +11456,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B21">
-    <cfRule type="duplicateValues" dxfId="3" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A21">
-    <cfRule type="duplicateValues" dxfId="2" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{00000000-0002-0000-6200-000000000000}">
@@ -12727,10 +12717,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="367" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="366" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="366" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="365" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12831,19 +12821,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="365" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="364" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="364" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="363" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="363" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="362" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="362" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="361" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" dxfId="361" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="360" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
@@ -12908,10 +12898,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="duplicateValues" dxfId="360" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="359" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="359" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="358" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
@@ -12982,16 +12972,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="duplicateValues" dxfId="358" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="357" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="357" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="356" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="356" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="355" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="355" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="354" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
@@ -13062,10 +13052,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="duplicateValues" dxfId="354" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="353" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="353" priority="169"/>
+    <cfRule type="duplicateValues" dxfId="352" priority="169"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
@@ -13197,13 +13187,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="352" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="351" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="351" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="350" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="350" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="349" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
@@ -13258,10 +13248,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="349" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="348" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="348" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="347" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0F00-000000000000}">
@@ -13315,10 +13305,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="347" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="346" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="346" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="345" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13371,9 +13361,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AT102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B5" sqref="B5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15"/>
@@ -17323,178 +17313,178 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="529" priority="80"/>
+    <cfRule type="duplicateValues" dxfId="528" priority="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51:B52">
-    <cfRule type="duplicateValues" dxfId="528" priority="78"/>
+    <cfRule type="duplicateValues" dxfId="527" priority="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="527" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="526" priority="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="duplicateValues" dxfId="526" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="525" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="duplicateValues" dxfId="525" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="524" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="duplicateValues" dxfId="524" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="523" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74">
-    <cfRule type="duplicateValues" dxfId="523" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="522" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="duplicateValues" dxfId="522" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="521" priority="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="duplicateValues" dxfId="521" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="520" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79">
-    <cfRule type="duplicateValues" dxfId="520" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="519" priority="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="duplicateValues" dxfId="519" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="518" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="duplicateValues" dxfId="518" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="517" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="duplicateValues" dxfId="517" priority="61"/>
+    <cfRule type="duplicateValues" dxfId="516" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="duplicateValues" dxfId="516" priority="60"/>
+    <cfRule type="duplicateValues" dxfId="515" priority="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="duplicateValues" dxfId="515" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="514" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="duplicateValues" dxfId="514" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="513" priority="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76">
-    <cfRule type="duplicateValues" dxfId="513" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="512" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77">
-    <cfRule type="duplicateValues" dxfId="512" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="511" priority="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="duplicateValues" dxfId="511" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="510" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79">
-    <cfRule type="duplicateValues" dxfId="510" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="509" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B104:B1048576 B102 B55:B57 B59:B62 B67:B68 B71:B74 B77:B83 B33:B49 B1:B31">
-    <cfRule type="duplicateValues" dxfId="509" priority="123"/>
+    <cfRule type="duplicateValues" dxfId="508" priority="123"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72">
-    <cfRule type="duplicateValues" dxfId="508" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="507" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="duplicateValues" dxfId="507" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="506" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="duplicateValues" dxfId="506" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="505" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D86">
-    <cfRule type="duplicateValues" dxfId="505" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="504" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87:B91">
-    <cfRule type="duplicateValues" dxfId="504" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="503" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="duplicateValues" dxfId="503" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="502" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87:D90">
-    <cfRule type="duplicateValues" dxfId="502" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="501" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92">
-    <cfRule type="duplicateValues" dxfId="501" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="500" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D91">
-    <cfRule type="duplicateValues" dxfId="500" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="499" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="duplicateValues" dxfId="499" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="498" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="duplicateValues" dxfId="498" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="497" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D84">
-    <cfRule type="duplicateValues" dxfId="497" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="496" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D97">
-    <cfRule type="duplicateValues" dxfId="496" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="495" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97">
-    <cfRule type="duplicateValues" dxfId="495" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="494" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G97:I97">
-    <cfRule type="duplicateValues" dxfId="494" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="493" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="duplicateValues" dxfId="493" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="492" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99">
-    <cfRule type="duplicateValues" dxfId="492" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="491" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="491" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="490" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100:B101">
-    <cfRule type="duplicateValues" dxfId="490" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="489" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D100">
-    <cfRule type="duplicateValues" dxfId="489" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="488" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D101">
-    <cfRule type="duplicateValues" dxfId="488" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="487" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98">
-    <cfRule type="duplicateValues" dxfId="487" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="486" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="duplicateValues" dxfId="486" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="485" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="duplicateValues" dxfId="485" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="484" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="duplicateValues" dxfId="484" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="483" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="duplicateValues" dxfId="483" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="482" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="duplicateValues" dxfId="482" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="481" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="duplicateValues" dxfId="481" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="480" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="duplicateValues" dxfId="480" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="479" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
-    <cfRule type="duplicateValues" dxfId="479" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="478" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
-    <cfRule type="duplicateValues" dxfId="478" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="477" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69">
-    <cfRule type="duplicateValues" dxfId="477" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="476" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
-    <cfRule type="duplicateValues" dxfId="476" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="475" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="duplicateValues" dxfId="475" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="474" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="474" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="473" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85">
-    <cfRule type="duplicateValues" dxfId="473" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="472" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="duplicateValues" dxfId="472" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="471" priority="5"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="I3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -17861,6 +17851,8 @@
     <hyperlink ref="H82" location="'icVerifyForgotPass++'!A1" display="icVerifyForgotPass" xr:uid="{3FEF4908-3C4A-4A8F-966B-E17081D1E2E1}"/>
     <hyperlink ref="I68" location="'icVerifyForgotPass++'!A1" display="icVerifyForgotPass" xr:uid="{C51CD10E-5A7E-4A0F-B562-F6C24AC47DC3}"/>
     <hyperlink ref="H86" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{B10485F2-5D33-42F9-8035-38D1AC21BA5C}"/>
+    <hyperlink ref="I7" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{03A3E7FF-424C-4EF1-A086-37208C55FE82}"/>
+    <hyperlink ref="I8:I15" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{F42EBB57-3878-4432-B853-0A860011A6DF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -17914,7 +17906,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="345" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="344" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
@@ -17982,10 +17974,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="344" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="343" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="343" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="342" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
@@ -18578,7 +18570,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B14:B18">
-    <cfRule type="duplicateValues" dxfId="342" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="341" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18" xr:uid="{00000000-0002-0000-1500-000000000000}">
@@ -18866,31 +18858,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:A7">
-    <cfRule type="duplicateValues" dxfId="341" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="340" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="340" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="339" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="339" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="338" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="duplicateValues" dxfId="338" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="337" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="337" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="336" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="336" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="335" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="335" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="334" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="334" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="333" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="333" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="332" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
@@ -19246,34 +19238,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A7:A8">
-    <cfRule type="duplicateValues" dxfId="332" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="331" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="331" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="330" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="330" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="329" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A13">
-    <cfRule type="duplicateValues" dxfId="329" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="328" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="328" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="327" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="327" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="326" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="326" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="325" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="325" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="324" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="324" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="323" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="323" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="322" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
@@ -20015,46 +20007,46 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B15">
-    <cfRule type="duplicateValues" dxfId="322" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="321" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:B25">
-    <cfRule type="duplicateValues" dxfId="321" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="320" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:A36">
-    <cfRule type="duplicateValues" dxfId="320" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="319" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="duplicateValues" dxfId="319" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="318" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="318" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="317" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:A41">
-    <cfRule type="duplicateValues" dxfId="317" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="316" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="duplicateValues" dxfId="316" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="315" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="duplicateValues" dxfId="315" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="314" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:A43">
-    <cfRule type="duplicateValues" dxfId="314" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="313" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="duplicateValues" dxfId="313" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="312" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="duplicateValues" dxfId="312" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="311" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B31">
-    <cfRule type="duplicateValues" dxfId="311" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="310" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="duplicateValues" dxfId="310" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="309" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="duplicateValues" dxfId="309" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="308" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
@@ -20774,34 +20766,34 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B33:B35">
-    <cfRule type="duplicateValues" dxfId="308" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="307" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="duplicateValues" dxfId="307" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="306" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="306" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="305" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A32">
-    <cfRule type="duplicateValues" dxfId="305" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="304" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B32">
-    <cfRule type="duplicateValues" dxfId="304" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="303" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="303" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="302" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:B43">
-    <cfRule type="duplicateValues" dxfId="302" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="301" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="duplicateValues" dxfId="301" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="300" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="duplicateValues" dxfId="300" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="299" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="duplicateValues" dxfId="299" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="298" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
@@ -20888,7 +20880,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="298" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="297" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21795,61 +21787,61 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="297" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="296" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:B28">
-    <cfRule type="duplicateValues" dxfId="296" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="295" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B26">
-    <cfRule type="duplicateValues" dxfId="295" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="294" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="duplicateValues" dxfId="294" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="293" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="duplicateValues" dxfId="293" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="292" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="duplicateValues" dxfId="292" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="291" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="duplicateValues" dxfId="291" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="290" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="duplicateValues" dxfId="290" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="289" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="duplicateValues" dxfId="289" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="288" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="duplicateValues" dxfId="288" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="287" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="duplicateValues" dxfId="287" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="286" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="duplicateValues" dxfId="286" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="285" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="duplicateValues" dxfId="285" priority="189"/>
+    <cfRule type="duplicateValues" dxfId="284" priority="189"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="duplicateValues" dxfId="284" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="283" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="duplicateValues" dxfId="283" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="282" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61:B62">
-    <cfRule type="duplicateValues" dxfId="282" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="281" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="duplicateValues" dxfId="281" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="280" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:B51 B18:B23 B2:B16 B29:B44">
-    <cfRule type="duplicateValues" dxfId="280" priority="191"/>
+    <cfRule type="duplicateValues" dxfId="279" priority="191"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A55">
-    <cfRule type="duplicateValues" dxfId="279" priority="195"/>
+    <cfRule type="duplicateValues" dxfId="278" priority="195"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1B00-000000000000}">
@@ -25639,172 +25631,172 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="471" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="470" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="470" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="469" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="469" priority="95"/>
+    <cfRule type="duplicateValues" dxfId="468" priority="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D7">
-    <cfRule type="duplicateValues" dxfId="468" priority="94"/>
+    <cfRule type="duplicateValues" dxfId="467" priority="94"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="467" priority="188"/>
+    <cfRule type="duplicateValues" dxfId="466" priority="188"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="466" priority="81"/>
+    <cfRule type="duplicateValues" dxfId="465" priority="81"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="465" priority="80"/>
+    <cfRule type="duplicateValues" dxfId="464" priority="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="464" priority="78"/>
+    <cfRule type="duplicateValues" dxfId="463" priority="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D13 D15:D23">
-    <cfRule type="duplicateValues" dxfId="463" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="462" priority="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:D32">
-    <cfRule type="duplicateValues" dxfId="462" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="461" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B32">
-    <cfRule type="duplicateValues" dxfId="461" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="460" priority="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:D37">
-    <cfRule type="duplicateValues" dxfId="460" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="459" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:B37">
-    <cfRule type="duplicateValues" dxfId="459" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="458" priority="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="458" priority="72"/>
+    <cfRule type="duplicateValues" dxfId="457" priority="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="457" priority="71"/>
+    <cfRule type="duplicateValues" dxfId="456" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:B42">
-    <cfRule type="duplicateValues" dxfId="456" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="455" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="duplicateValues" dxfId="455" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="454" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="duplicateValues" dxfId="454" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="453" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="duplicateValues" dxfId="453" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="452" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="duplicateValues" dxfId="452" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="451" priority="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="duplicateValues" dxfId="451" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="450" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="duplicateValues" dxfId="450" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="449" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54:B55">
-    <cfRule type="duplicateValues" dxfId="449" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="448" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54">
-    <cfRule type="duplicateValues" dxfId="448" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="447" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="duplicateValues" dxfId="447" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="446" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="duplicateValues" dxfId="446" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="445" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="duplicateValues" dxfId="445" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="444" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="duplicateValues" dxfId="444" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="443" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="duplicateValues" dxfId="443" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="442" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="duplicateValues" dxfId="442" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="441" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="duplicateValues" dxfId="441" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="440" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
-    <cfRule type="duplicateValues" dxfId="440" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="439" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
-    <cfRule type="duplicateValues" dxfId="439" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="438" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72">
-    <cfRule type="duplicateValues" dxfId="438" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="437" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71">
-    <cfRule type="duplicateValues" dxfId="437" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="436" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73">
-    <cfRule type="duplicateValues" dxfId="436" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="435" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74:B75">
-    <cfRule type="duplicateValues" dxfId="435" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="434" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74:D75">
-    <cfRule type="duplicateValues" dxfId="434" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="433" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="433" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="432" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="432" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="431" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="duplicateValues" dxfId="431" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="430" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:B51">
-    <cfRule type="duplicateValues" dxfId="430" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="429" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47:G50 I47:I50">
-    <cfRule type="duplicateValues" dxfId="429" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="428" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="duplicateValues" dxfId="428" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="427" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47:D50">
-    <cfRule type="duplicateValues" dxfId="427" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="426" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51:H52">
-    <cfRule type="duplicateValues" dxfId="426" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="425" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="duplicateValues" dxfId="425" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="424" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="duplicateValues" dxfId="424" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="423" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="duplicateValues" dxfId="423" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="422" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77">
-    <cfRule type="duplicateValues" dxfId="422" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="421" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G77 I77">
-    <cfRule type="duplicateValues" dxfId="421" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="420" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79">
-    <cfRule type="duplicateValues" dxfId="420" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="419" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B81">
-    <cfRule type="duplicateValues" dxfId="419" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="418" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82">
-    <cfRule type="duplicateValues" dxfId="418" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="417" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67:W67">
-    <cfRule type="duplicateValues" dxfId="417" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="416" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67">
-    <cfRule type="duplicateValues" dxfId="416" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="415" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H2" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -26315,10 +26307,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="278" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="277" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="277" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="276" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1F00-000000000000}">
@@ -26644,10 +26636,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="276" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="275" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B18">
-    <cfRule type="duplicateValues" dxfId="275" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="274" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D21" xr:uid="{00000000-0002-0000-2000-000000000000}">
@@ -26783,10 +26775,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="274" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="273" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="273" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="272" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
@@ -26864,10 +26856,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="272" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="271" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="271" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="270" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="automation13@gmail.com" xr:uid="{00000000-0004-0000-2300-000000000000}"/>
@@ -26954,7 +26946,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="270" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="269" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27067,22 +27059,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="269" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="268" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="268" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="267" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="duplicateValues" dxfId="267" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="266" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="266" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="265" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="265" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="264" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="264" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="263" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
@@ -27368,25 +27360,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="263" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="262" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="262" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="261" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4 B6">
-    <cfRule type="duplicateValues" dxfId="261" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="260" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="260" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="259" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="259" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="258" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="258" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="257" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="257" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="256" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9" xr:uid="{00000000-0002-0000-2600-000000000000}">
@@ -27610,19 +27602,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="256" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="255" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="255" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="254" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="duplicateValues" dxfId="254" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="253" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="253" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="252" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="252" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="251" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2:E3" r:id="rId1" display="watlevi41@gmail.com" xr:uid="{00000000-0004-0000-2700-000000000000}"/>
@@ -27973,7 +27965,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="251" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="250" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R8" xr:uid="{00000000-0002-0000-2800-000000000000}">
@@ -28380,7 +28372,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="250" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="249" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-2A00-000000000000}"/>
@@ -28482,7 +28474,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="249" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="248" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-2B00-000000000000}">
@@ -28758,31 +28750,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A7:A8">
-    <cfRule type="duplicateValues" dxfId="248" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="247" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="247" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="246" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="246" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="245" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A13">
-    <cfRule type="duplicateValues" dxfId="245" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="244" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="244" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="243" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="243" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="242" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="242" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="241" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="241" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="240" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="240" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="239" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2C00-000000000000}"/>
@@ -29349,31 +29341,31 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A5:A6">
-    <cfRule type="duplicateValues" dxfId="239" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="238" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="238" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="237" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="237" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="236" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A11">
-    <cfRule type="duplicateValues" dxfId="236" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="235" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="235" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="234" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="234" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="233" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="233" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="232" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="232" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="231" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="231" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="230" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2D00-000000000000}"/>
@@ -29696,31 +29688,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A7:A8">
-    <cfRule type="duplicateValues" dxfId="230" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="229" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="229" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="228" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="228" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="227" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A13">
-    <cfRule type="duplicateValues" dxfId="227" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="226" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="226" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="225" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="225" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="224" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="224" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="223" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="223" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="222" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="222" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="221" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D16 D2 D19:D20" xr:uid="{00000000-0002-0000-2E00-000000000000}">
@@ -30098,34 +30090,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="221" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="220" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A8">
-    <cfRule type="duplicateValues" dxfId="220" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="219" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="219" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="218" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="218" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="217" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A13">
-    <cfRule type="duplicateValues" dxfId="217" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="216" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="216" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="215" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="215" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="214" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="214" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="213" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="213" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="212" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="212" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="211" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2F00-000000000000}"/>
@@ -30180,7 +30172,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="415" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="414" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -31125,22 +31117,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="211" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="210" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="210" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="209" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A11">
-    <cfRule type="duplicateValues" dxfId="209" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="208" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="208" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="207" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="207" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="206" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="206" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="205" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-3000-000000000000}"/>
@@ -31925,7 +31917,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B16:B20">
-    <cfRule type="duplicateValues" dxfId="205" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="204" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q21:R22 P7 P2:T3 P10:P1048576 T7:T10 Q11:R17 S11:S15" xr:uid="{00000000-0002-0000-3100-000000000000}">
@@ -33357,82 +33349,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="204" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="203" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="203" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="202" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="202" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="201" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="201" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="200" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="200" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="199" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="199" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="198" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="198" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="197" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="197" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="196" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="196" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="195" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="195" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="194" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="duplicateValues" dxfId="194" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="193" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="193" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="192" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="192" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="191" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="duplicateValues" dxfId="191" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="190" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="190" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="189" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:A28">
-    <cfRule type="duplicateValues" dxfId="189" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="188" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="188" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="187" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="duplicateValues" dxfId="187" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="186" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:A31">
-    <cfRule type="duplicateValues" dxfId="186" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="185" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="duplicateValues" dxfId="185" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="184" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="duplicateValues" dxfId="184" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="183" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="183" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="182" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="182" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="181" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="181" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="180" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="duplicateValues" dxfId="180" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="179" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="duplicateValues" dxfId="179" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="178" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G21 G23:G29 G33:G39" xr:uid="{00000000-0002-0000-3200-000000000000}">
@@ -35091,52 +35083,52 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B15">
-    <cfRule type="duplicateValues" dxfId="178" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="177" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="177" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="176" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="duplicateValues" dxfId="176" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="175" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="175" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="174" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B33">
-    <cfRule type="duplicateValues" dxfId="174" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="173" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="173" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="172" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="172" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="171" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="duplicateValues" dxfId="171" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="170" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="170" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="duplicateValues" dxfId="169" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="168" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="167" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="duplicateValues" dxfId="167" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="166" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:B44">
-    <cfRule type="duplicateValues" dxfId="166" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="duplicateValues" dxfId="165" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="164" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="163" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H16" xr:uid="{00000000-0002-0000-3300-000000000000}">
@@ -36422,22 +36414,22 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A27">
-    <cfRule type="duplicateValues" dxfId="163" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="162" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="160" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B31">
-    <cfRule type="duplicateValues" dxfId="161" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="159" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A31">
-    <cfRule type="duplicateValues" dxfId="160" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B26">
-    <cfRule type="duplicateValues" dxfId="159" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A26">
-    <cfRule type="duplicateValues" dxfId="158" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="68"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M32" xr:uid="{00000000-0002-0000-3400-000000000000}">
@@ -36548,7 +36540,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="157" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-3500-000000000000}"/>
@@ -37056,64 +37048,64 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B4">
-    <cfRule type="duplicateValues" dxfId="156" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="155" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="154" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B13">
-    <cfRule type="duplicateValues" dxfId="153" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="152" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="151" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B17">
-    <cfRule type="duplicateValues" dxfId="150" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="149" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="148" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="147" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="146" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="145" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="144" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="143" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="duplicateValues" dxfId="142" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="duplicateValues" dxfId="141" priority="169"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="169"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="duplicateValues" dxfId="140" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="139" priority="170"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="170"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="duplicateValues" dxfId="138" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="duplicateValues" dxfId="137" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-3600-000000000000}"/>
@@ -37357,13 +37349,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B5">
-    <cfRule type="duplicateValues" dxfId="136" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="135" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="134" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-3700-000000000000}"/>
@@ -37600,16 +37592,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B5">
-    <cfRule type="duplicateValues" dxfId="133" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="132" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="131" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="130" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37742,13 +37734,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="414" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="413" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="413" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="412" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="412" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="411" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37903,13 +37895,13 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="129" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="128" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="127" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38060,16 +38052,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2 B4">
-    <cfRule type="duplicateValues" dxfId="126" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2 A4">
-    <cfRule type="duplicateValues" dxfId="125" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="124" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="123" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-3C00-000000000000}">
@@ -38390,13 +38382,13 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="122" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="121" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="120" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8" xr:uid="{00000000-0002-0000-3D00-000000000000}">
@@ -38421,9 +38413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -38792,22 +38782,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A21">
-    <cfRule type="duplicateValues" dxfId="119" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="duplicateValues" dxfId="118" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="117" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="116" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A26">
-    <cfRule type="duplicateValues" dxfId="115" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B26">
-    <cfRule type="duplicateValues" dxfId="114" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3E00-000000000000}">
@@ -38904,7 +38894,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="113" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38964,10 +38954,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="112" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="111" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39124,10 +39114,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="110" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="109" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-4100-000000000000}">
@@ -39252,10 +39242,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="108" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="107" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-4200-000000000000}">
@@ -39404,10 +39394,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="106" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="105" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-4300-000000000000}">
@@ -39477,7 +39467,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="411" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="410" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -39592,10 +39582,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="104" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="103" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-4400-000000000000}">
@@ -39848,10 +39838,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="102" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="101" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3" xr:uid="{00000000-0002-0000-4500-000000000000}">
@@ -39943,10 +39933,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="100" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="99" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39998,10 +39988,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="98" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="97" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -40729,22 +40719,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="96" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="95" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="94" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="93" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="92" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="91" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="89" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10" xr:uid="{00000000-0002-0000-4900-000000000000}">
@@ -41405,22 +41395,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="90" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="89" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="88" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="87" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="86" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="85" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576" xr:uid="{00000000-0002-0000-4A00-000000000000}">
@@ -41880,10 +41870,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="84" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="83" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-4B00-000000000000}">
@@ -42542,22 +42532,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="duplicateValues" dxfId="82" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="81" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="80" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="79" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="78" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4C00-000000000000}"/>
@@ -42922,28 +42912,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="76" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="75" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="74" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="73" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="72" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="71" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:B23">
-    <cfRule type="duplicateValues" dxfId="70" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-4D00-000000000000}">
@@ -43931,118 +43921,118 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="410" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="409" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="409" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="408" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="408" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="407" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="407" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="406" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="406" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="405" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B27">
-    <cfRule type="duplicateValues" dxfId="405" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="404" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="duplicateValues" dxfId="404" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="403" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="403" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="402" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B32">
-    <cfRule type="duplicateValues" dxfId="402" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="401" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="duplicateValues" dxfId="401" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="400" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="duplicateValues" dxfId="400" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="399" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="duplicateValues" dxfId="399" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="398" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="398" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="397" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="duplicateValues" dxfId="397" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="396" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="396" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="395" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="395" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="394" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40:B41">
-    <cfRule type="duplicateValues" dxfId="394" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="393" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48">
-    <cfRule type="duplicateValues" dxfId="393" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="392" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="duplicateValues" dxfId="392" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="391" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="duplicateValues" dxfId="391" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="390" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="duplicateValues" dxfId="390" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="389" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="duplicateValues" dxfId="389" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="388" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="duplicateValues" dxfId="388" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="387" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="duplicateValues" dxfId="387" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="386" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="duplicateValues" dxfId="386" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="385" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="duplicateValues" dxfId="385" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="384" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50">
-    <cfRule type="duplicateValues" dxfId="384" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="383" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="duplicateValues" dxfId="383" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="382" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:A52">
-    <cfRule type="duplicateValues" dxfId="382" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="381" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="duplicateValues" dxfId="381" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="380" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="duplicateValues" dxfId="380" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="379" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="duplicateValues" dxfId="379" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="378" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="duplicateValues" dxfId="378" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="377" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="duplicateValues" dxfId="377" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="376" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="duplicateValues" dxfId="376" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="375" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="duplicateValues" dxfId="375" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="374" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="duplicateValues" dxfId="374" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="373" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
-    <cfRule type="duplicateValues" dxfId="373" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="372" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0600-000000000000}">
@@ -45315,28 +45305,28 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="duplicateValues" dxfId="68" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="67" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B33">
-    <cfRule type="duplicateValues" dxfId="66" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A33">
-    <cfRule type="duplicateValues" dxfId="65" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="64" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="duplicateValues" dxfId="63" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:B42">
-    <cfRule type="duplicateValues" dxfId="62" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="61" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-4E00-000000000000}"/>
@@ -45515,16 +45505,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="60" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="duplicateValues" dxfId="59" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B12">
-    <cfRule type="duplicateValues" dxfId="58" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A12">
-    <cfRule type="duplicateValues" dxfId="57" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -46006,19 +45996,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="56" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A13">
-    <cfRule type="duplicateValues" dxfId="55" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="54" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="53" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-5100-000000000000}"/>
@@ -46408,22 +46398,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="51" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="50" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="49" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="48" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="47" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-5200-000000000000}"/>
@@ -46838,22 +46828,22 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="45" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="44" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="43" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="42" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="41" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-5300-000000000000}"/>
@@ -47160,34 +47150,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="39" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="38" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="37" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="36" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="35" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="34" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="33" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="32" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="31" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-5400-000000000000}"/>
@@ -48301,34 +48291,34 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="duplicateValues" dxfId="29" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="duplicateValues" dxfId="28" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="duplicateValues" dxfId="27" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B21">
-    <cfRule type="duplicateValues" dxfId="26" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="25" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="24" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="duplicateValues" dxfId="23" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="duplicateValues" dxfId="22" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-5900-000000000000}"/>
@@ -48605,31 +48595,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9:B12">
-    <cfRule type="duplicateValues" dxfId="19" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A12">
-    <cfRule type="duplicateValues" dxfId="18" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="17" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B7">
-    <cfRule type="duplicateValues" dxfId="16" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="15" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="14" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-5A00-000000000000}"/>
@@ -48732,13 +48722,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="10" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-5B00-000000000000}"/>

</xml_diff>